<commit_message>
Css styles and excel reader fix
</commit_message>
<xml_diff>
--- a/proba.xlsx
+++ b/proba.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dariusz\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFC2EE7-30B4-4D45-9BF6-E8AE2FA065C9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2F0ADD-223B-4CB4-A08B-23A0FA99BBEB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9105" xr2:uid="{7ADF90F3-0A3C-42F9-A9C4-9580D444B114}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>L</t>
   </si>
@@ -54,49 +54,70 @@
     <t>60</t>
   </si>
   <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>dr.inz.</t>
-  </si>
-  <si>
-    <t>Przedmiot 1</t>
-  </si>
-  <si>
-    <t>Imie</t>
-  </si>
-  <si>
-    <t>Naziwsko</t>
-  </si>
-  <si>
-    <t>Imie1</t>
-  </si>
-  <si>
-    <t>Naziwsko1</t>
-  </si>
-  <si>
-    <t>Imie2</t>
-  </si>
-  <si>
-    <t>Naziwsko2</t>
-  </si>
-  <si>
-    <t>Przedmiot 2</t>
-  </si>
-  <si>
-    <t>Imie3</t>
-  </si>
-  <si>
-    <t>Naziwsko3</t>
+    <t>Programowanie Mobilne</t>
+  </si>
+  <si>
+    <t>dr hab.</t>
+  </si>
+  <si>
+    <t>Joanna</t>
+  </si>
+  <si>
+    <t>Kołodziej</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>Andrzej</t>
+  </si>
+  <si>
+    <t>mgr inż.</t>
+  </si>
+  <si>
+    <t>Wilczyński</t>
+  </si>
+  <si>
+    <t>Automaty Języki i Obliczenia</t>
+  </si>
+  <si>
+    <t>dr inż.</t>
+  </si>
+  <si>
+    <t>Jerzy</t>
+  </si>
+  <si>
+    <t>Zaczek</t>
+  </si>
+  <si>
+    <t>Architektura Systemów Komputerowych</t>
+  </si>
+  <si>
+    <t>Tomasz</t>
+  </si>
+  <si>
+    <t>Sośnicki</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>Michał</t>
+  </si>
+  <si>
+    <t>Niedźwiecki</t>
+  </si>
+  <si>
+    <t>Przetwarzanie Języka Naturalnego</t>
+  </si>
+  <si>
+    <t>Krzysztof</t>
+  </si>
+  <si>
+    <t>Rzecki</t>
   </si>
 </sst>
 </file>
@@ -451,17 +472,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F17039-7E08-46B8-8CC7-9AE4422E17DA}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
     <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
@@ -485,16 +506,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -503,100 +524,163 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed problem with window resizing
</commit_message>
<xml_diff>
--- a/proba.xlsx
+++ b/proba.xlsx
@@ -1,37 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dariusz\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2F0ADD-223B-4CB4-A08B-23A0FA99BBEB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E88879-BC42-48C1-AB4A-AEB3FDEAE0B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9105" xr2:uid="{7ADF90F3-0A3C-42F9-A9C4-9580D444B114}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{7ADF90F3-0A3C-42F9-A9C4-9580D444B114}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>L</t>
   </si>
@@ -118,6 +112,15 @@
   </si>
   <si>
     <t>Rzecki</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,10 +585,10 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>5</v>
@@ -666,6 +669,9 @@
       </c>
       <c r="D15" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
spring security done + 403 template
</commit_message>
<xml_diff>
--- a/proba.xlsx
+++ b/proba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dariusz\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E88879-BC42-48C1-AB4A-AEB3FDEAE0B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A3038C-CC36-4673-AA19-0194EB459695}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{7ADF90F3-0A3C-42F9-A9C4-9580D444B114}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="23280" windowHeight="12720" xr2:uid="{7ADF90F3-0A3C-42F9-A9C4-9580D444B114}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -157,9 +157,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -478,7 +477,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,10 +499,10 @@
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -514,11 +513,11 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -535,18 +534,18 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="D4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -555,10 +554,10 @@
       <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -572,12 +571,12 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D7" s="2"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -587,10 +586,10 @@
       <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -604,12 +603,12 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D10" s="2"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -618,10 +617,10 @@
       <c r="B11" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -635,7 +634,7 @@
       <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="1"/>
@@ -650,12 +649,12 @@
       <c r="C13" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D14" s="2"/>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -664,10 +663,10 @@
       <c r="B15" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E15" t="s">
@@ -684,7 +683,7 @@
       <c r="C16" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>